<commit_message>
test: Add mock data for prompt payment report
</commit_message>
<xml_diff>
--- a/app/tests/integration_tests/prompt_payment/new_report_input.xlsx
+++ b/app/tests/integration_tests/prompt_payment/new_report_input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdaly/Documents/PyProjects/py3.7.7/DGS/priority-vendor-aging-report/app/tests/unit_tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdaly/Documents/PyProjects/py3.7.7/DGS/priority-vendor-aging-report/app/tests/integration_tests/prompt_payment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79A36617-52A9-324A-B5DC-09CD18FFFB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2351BA-B5D2-C647-8635-2F368A24B65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28560" windowHeight="12920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>Execution ID</t>
   </si>
@@ -87,9 +87,6 @@
     <t>EA Invoice Approval</t>
   </si>
   <si>
-    <t>Erica Turner</t>
-  </si>
-  <si>
     <t>1851</t>
   </si>
   <si>
@@ -108,18 +105,12 @@
     <t>1929</t>
   </si>
   <si>
-    <t>Melody Bailey</t>
-  </si>
-  <si>
     <t>9213290241</t>
   </si>
   <si>
     <t>06/24/2019</t>
   </si>
   <si>
-    <t>Tiffany Lowery</t>
-  </si>
-  <si>
     <t>2019-4-32819</t>
   </si>
   <si>
@@ -129,9 +120,6 @@
     <t>DGS - CitiBuy</t>
   </si>
   <si>
-    <t>Rosa Gold</t>
-  </si>
-  <si>
     <t>107082</t>
   </si>
   <si>
@@ -171,9 +159,6 @@
     <t>John Doe</t>
   </si>
   <si>
-    <t>Lakia Carrillo</t>
-  </si>
-  <si>
     <t>Disney</t>
   </si>
   <si>
@@ -202,6 +187,15 @@
   </si>
   <si>
     <t>Google</t>
+  </si>
+  <si>
+    <t>Mickey Mouse</t>
+  </si>
+  <si>
+    <t>Donald Duck</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
   </si>
 </sst>
 </file>
@@ -607,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92038BFC-ECD5-DD41-99FF-9C3ACD1E6055}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -683,7 +677,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>1056</v>
@@ -692,7 +686,7 @@
         <v>1455</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2">
         <v>10.11</v>
@@ -701,28 +695,28 @@
         <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="I2">
         <v>43046.647809294001</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
       <c r="N2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.15">
@@ -731,7 +725,7 @@
         <v>2227125</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3">
         <v>939</v>
@@ -740,7 +734,7 @@
         <v>949</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3">
         <v>20.22</v>
@@ -749,28 +743,28 @@
         <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="I3">
         <v>43552.615498148101</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="O3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.15">
@@ -779,7 +773,7 @@
         <v>2279092</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>164</v>
@@ -788,40 +782,40 @@
         <v>852</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>30.33</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="I4">
         <v>43649.710519560198</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="O4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
@@ -830,7 +824,7 @@
         <v>2285692</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>838</v>
@@ -848,28 +842,28 @@
         <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="I5">
         <v>43663.584528784697</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="O5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
@@ -878,7 +872,7 @@
         <v>2601862</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>60</v>
@@ -887,40 +881,40 @@
         <v>398</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="I6">
         <v>44103.674299999999</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="L6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="O6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
@@ -929,7 +923,7 @@
         <v>2688291</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>28</v>
@@ -938,40 +932,40 @@
         <v>222</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7">
         <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I7">
         <v>44279.888816435203</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="N7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="O7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -989,6 +983,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D7CE14B07C41F44A983E091F6E80062E" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29159d5a7bc3713cc8dad0f30b0a42a0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4b30ab28-39cc-41c9-a02b-b53b4cc9e5a7" xmlns:ns3="dc3378cc-208d-46dc-bcc8-e7d1802d44a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0ecefbf6125b54a2f3c4950064a5ba3" ns2:_="" ns3:_="">
     <xsd:import namespace="4b30ab28-39cc-41c9-a02b-b53b4cc9e5a7"/>
@@ -1165,12 +1165,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AA5E1D7-B7CD-45BD-9547-2DBA0FF1AB7B}">
   <ds:schemaRefs>
@@ -1180,6 +1174,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1603A941-D14B-470C-9D1B-A062CB1C4DF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE8AF8A5-7563-4C8D-91A1-6EB455D01FE2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1196,13 +1199,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1603A941-D14B-470C-9D1B-A062CB1C4DF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>